<commit_message>
Update Optostim Receiver BOM.xlsx
</commit_message>
<xml_diff>
--- a/PWMpulsebox v2 PCB/Optostim Receiver BOM.xlsx
+++ b/PWMpulsebox v2 PCB/Optostim Receiver BOM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>Country of Origin may be different at time of shipment.</t>
   </si>
@@ -215,6 +215,18 @@
     <t>1,009</t>
   </si>
   <si>
+    <t>Tube</t>
+  </si>
+  <si>
+    <t>2223-DS01C-254-L-03BE-ND</t>
+  </si>
+  <si>
+    <t>0.57000</t>
+  </si>
+  <si>
+    <t>$0.57</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
@@ -245,6 +257,15 @@
     <t>1,683</t>
   </si>
   <si>
+    <t>A123828-ND</t>
+  </si>
+  <si>
+    <t>2.41000</t>
+  </si>
+  <si>
+    <t>$2.41</t>
+  </si>
+  <si>
     <t>39</t>
   </si>
   <si>
@@ -269,6 +290,18 @@
     <t>285,237</t>
   </si>
   <si>
+    <t>Cut Tape (CT)</t>
+  </si>
+  <si>
+    <t>CR0805-FX-4701ELFCT-ND</t>
+  </si>
+  <si>
+    <t>0.10000</t>
+  </si>
+  <si>
+    <t>$0.30</t>
+  </si>
+  <si>
     <t>15</t>
   </si>
   <si>
@@ -299,6 +332,15 @@
     <t>6,450</t>
   </si>
   <si>
+    <t>360-3252-ND</t>
+  </si>
+  <si>
+    <t>4.97000</t>
+  </si>
+  <si>
+    <t>$4.97</t>
+  </si>
+  <si>
     <t>22</t>
   </si>
   <si>
@@ -326,6 +368,15 @@
     <t>242</t>
   </si>
   <si>
+    <t>NCP1117ST50T3GOSCT-ND</t>
+  </si>
+  <si>
+    <t>0.72000</t>
+  </si>
+  <si>
+    <t>$0.72</t>
+  </si>
+  <si>
     <t>58</t>
   </si>
   <si>
@@ -356,6 +407,15 @@
     <t>2,792,077</t>
   </si>
   <si>
+    <t>1276-1052-1-ND</t>
+  </si>
+  <si>
+    <t>0.11000</t>
+  </si>
+  <si>
+    <t>$0.22</t>
+  </si>
+  <si>
     <t>https://www.samsungsem.com/kr/support/product-search/mlcc/CL21A106KPFNNNE.jsp</t>
   </si>
   <si>
@@ -377,6 +437,15 @@
     <t>92,528</t>
   </si>
   <si>
+    <t>CP-102A-ND</t>
+  </si>
+  <si>
+    <t>0.77000</t>
+  </si>
+  <si>
+    <t>$0.77</t>
+  </si>
+  <si>
     <t>https://www.cuidevices.com/product/resource/pj-102a.pdf</t>
   </si>
   <si>
@@ -392,7 +461,13 @@
     <t>RES SMD 1K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>1,555,528</t>
+    <t>1,558,028</t>
+  </si>
+  <si>
+    <t>CR0805-FX-1001ELFCT-ND</t>
+  </si>
+  <si>
+    <t>$0.10</t>
   </si>
   <si>
     <t>0731375003</t>
@@ -405,6 +480,15 @@
   </si>
   <si>
     <t>29,365</t>
+  </si>
+  <si>
+    <t>WM5514-ND</t>
+  </si>
+  <si>
+    <t>2.65000</t>
+  </si>
+  <si>
+    <t>$2.65</t>
   </si>
   <si>
     <t>12</t>
@@ -827,6 +911,27 @@
       <c r="F6" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="H6" s="0">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0">
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="0">
+        <v>1</v>
+      </c>
       <c r="O6" s="0" t="s">
         <v>40</v>
       </c>
@@ -834,16 +939,16 @@
         <v>64</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="S6" s="0" t="s">
         <v>40</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="U6" s="0" t="s">
         <v>40</v>
@@ -858,19 +963,19 @@
         <v>46</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="Z6" s="0" t="s">
         <v>48</v>
       </c>
       <c r="AA6" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AB6" s="0" t="s">
         <v>64</v>
       </c>
       <c r="AC6" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
@@ -878,37 +983,58 @@
         <v>4</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="H7" s="0">
+        <v>1</v>
+      </c>
+      <c r="I7" s="0">
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" s="0">
+        <v>1</v>
+      </c>
       <c r="O7" s="0" t="s">
         <v>40</v>
       </c>
       <c r="P7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="S7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>40</v>
@@ -917,7 +1043,7 @@
         <v>44</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="X7" s="0" t="s">
         <v>46</v>
@@ -932,10 +1058,10 @@
         <v>40</v>
       </c>
       <c r="AB7" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AC7" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
@@ -943,31 +1069,52 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="H8" s="0">
+        <v>3</v>
+      </c>
+      <c r="I8" s="0">
+        <v>3</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="N8" s="0">
+        <v>1</v>
+      </c>
       <c r="O8" s="0" t="s">
         <v>40</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="S8" s="0" t="s">
         <v>40</v>
@@ -988,19 +1135,19 @@
         <v>46</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="Z8" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB8" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="AA8" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB8" s="0" t="s">
-        <v>81</v>
-      </c>
       <c r="AC8" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9">
@@ -1008,31 +1155,52 @@
         <v>6</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="H9" s="0">
+        <v>1</v>
+      </c>
+      <c r="I9" s="0">
+        <v>1</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="N9" s="0">
+        <v>1</v>
+      </c>
       <c r="O9" s="0" t="s">
         <v>40</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="S9" s="0" t="s">
         <v>40</v>
@@ -1053,19 +1221,19 @@
         <v>46</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="AA9" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="AB9" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="AC9" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10">
@@ -1073,31 +1241,52 @@
         <v>7</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="H10" s="0">
+        <v>1</v>
+      </c>
+      <c r="I10" s="0">
+        <v>1</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="N10" s="0">
+        <v>1</v>
+      </c>
       <c r="O10" s="0" t="s">
         <v>40</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="S10" s="0" t="s">
         <v>40</v>
@@ -1118,19 +1307,19 @@
         <v>46</v>
       </c>
       <c r="Y10" s="0" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="AA10" s="0" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="AB10" s="0" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="AC10" s="0" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11">
@@ -1138,31 +1327,52 @@
         <v>8</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="H11" s="0">
+        <v>2</v>
+      </c>
+      <c r="I11" s="0">
+        <v>2</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="N11" s="0">
+        <v>1</v>
+      </c>
       <c r="O11" s="0" t="s">
         <v>40</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="S11" s="0" t="s">
         <v>40</v>
@@ -1183,19 +1393,19 @@
         <v>46</v>
       </c>
       <c r="Y11" s="0" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="Z11" s="0" t="s">
         <v>48</v>
       </c>
       <c r="AA11" s="0" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="AB11" s="0" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="AC11" s="0" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12">
@@ -1203,31 +1413,52 @@
         <v>9</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="H12" s="0">
+        <v>1</v>
+      </c>
+      <c r="I12" s="0">
+        <v>1</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="N12" s="0">
+        <v>1</v>
+      </c>
       <c r="O12" s="0" t="s">
         <v>40</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="Q12" s="0" t="s">
         <v>41</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="S12" s="0" t="s">
         <v>40</v>
@@ -1254,13 +1485,13 @@
         <v>48</v>
       </c>
       <c r="AA12" s="0" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="AB12" s="0" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="AC12" s="0" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13">
@@ -1268,31 +1499,52 @@
         <v>10</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="H13" s="0">
+        <v>1</v>
+      </c>
+      <c r="I13" s="0">
+        <v>1</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="N13" s="0">
+        <v>1</v>
+      </c>
       <c r="O13" s="0" t="s">
         <v>40</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="S13" s="0" t="s">
         <v>40</v>
@@ -1313,19 +1565,19 @@
         <v>46</v>
       </c>
       <c r="Y13" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="AA13" s="0" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="AB13" s="0" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="AC13" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14">
@@ -1333,31 +1585,52 @@
         <v>11</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="H14" s="0">
+        <v>1</v>
+      </c>
+      <c r="I14" s="0">
+        <v>1</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="N14" s="0">
+        <v>1</v>
+      </c>
       <c r="O14" s="0" t="s">
         <v>40</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="S14" s="0" t="s">
         <v>40</v>
@@ -1378,19 +1651,19 @@
         <v>46</v>
       </c>
       <c r="Y14" s="0" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="Z14" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="AA14" s="0" t="s">
         <v>40</v>
       </c>
       <c r="AB14" s="0" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="AC14" s="0" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15">
@@ -1398,16 +1671,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>35</v>
@@ -1422,13 +1695,13 @@
         <v>55</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="N15" s="0">
         <v>1</v>
@@ -1437,19 +1710,19 @@
         <v>40</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="S15" s="0" t="s">
         <v>40</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="U15" s="0" t="s">
         <v>40</v>
@@ -1464,7 +1737,7 @@
         <v>46</v>
       </c>
       <c r="Y15" s="0" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="Z15" s="0" t="s">
         <v>48</v>
@@ -1473,10 +1746,10 @@
         <v>40</v>
       </c>
       <c r="AB15" s="0" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="AC15" s="0" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16">
@@ -1484,19 +1757,19 @@
         <v>13</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="H16" s="0">
         <v>1</v>
@@ -1508,13 +1781,13 @@
         <v>55</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="N16" s="0">
         <v>1</v>
@@ -1523,13 +1796,13 @@
         <v>40</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="Q16" s="0" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="S16" s="0" t="s">
         <v>40</v>
@@ -1544,13 +1817,13 @@
         <v>44</v>
       </c>
       <c r="W16" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="X16" s="0" t="s">
         <v>46</v>
       </c>
       <c r="Y16" s="0" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="Z16" s="0" t="s">
         <v>62</v>
@@ -1559,10 +1832,10 @@
         <v>40</v>
       </c>
       <c r="AB16" s="0" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="AC16" s="0" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>